<commit_message>
Implementada función de Backup bi-direccional desde Firebase hacia Google Sheets
</commit_message>
<xml_diff>
--- a/Plantilla_Protesis.xlsx
+++ b/Plantilla_Protesis.xlsx
@@ -1,41 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Antigravity\Protesis COAT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+  </bookViews>
   <sheets>
     <sheet name="Protesis" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>FECHA RECEPCION</t>
+  </si>
+  <si>
+    <t>EMPRESA / OBRA SOCIAL</t>
+  </si>
+  <si>
+    <t>MEDICO</t>
+  </si>
+  <si>
+    <t>PACIENTE (APELLIDO Y NOMBRES)</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>TUBOS</t>
+  </si>
+  <si>
+    <t>RECIBE</t>
+  </si>
+  <si>
+    <t>NOTAS / OBSERVACIONES</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>FECHA COLOCACION</t>
+  </si>
+  <si>
+    <t>FECHA ENTREGA DOCS</t>
+  </si>
+  <si>
+    <t>ID FIREBASE (SISTEMA)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +98,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,143 +430,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="40.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="20.83203125" customWidth="1"/>
-    <col min="12" max="12" width="30.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="30.875" customWidth="1"/>
+    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="4" max="4" width="40.875" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="7" max="7" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="40.875" customWidth="1"/>
+    <col min="9" max="9" width="15.875" customWidth="1"/>
+    <col min="10" max="11" width="20.875" customWidth="1"/>
+    <col min="12" max="12" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>FECHA RECEPCION</v>
-      </c>
-      <c r="B1" t="str">
-        <v>EMPRESA / OBRA SOCIAL</v>
-      </c>
-      <c r="C1" t="str">
-        <v>MEDICO</v>
-      </c>
-      <c r="D1" t="str">
-        <v>PACIENTE (APELLIDO Y NOMBRES)</v>
-      </c>
-      <c r="E1" t="str">
-        <v>DNI</v>
-      </c>
-      <c r="F1" t="str">
-        <v>TUBOS</v>
-      </c>
-      <c r="G1" t="str">
-        <v>RECIBE</v>
-      </c>
-      <c r="H1" t="str">
-        <v>NOTAS / OBSERVACIONES</v>
-      </c>
-      <c r="I1" t="str">
-        <v>ESTADO</v>
-      </c>
-      <c r="J1" t="str">
-        <v>FECHA COLOCACION</v>
-      </c>
-      <c r="K1" t="str">
-        <v>FECHA ENTREGA DOCS</v>
-      </c>
-      <c r="L1" t="str">
-        <v>ID FIREBASE (SISTEMA)</v>
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2026-02-22</v>
-      </c>
-      <c r="B2" t="str">
-        <v>IMPLANTTECH</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Dr. Paredes</v>
-      </c>
-      <c r="D2" t="str">
-        <v>JUAN PEREZ</v>
-      </c>
-      <c r="E2" t="str">
-        <v>12345678</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Lujan</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Faltan tornillos</v>
-      </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2026-02-23</v>
-      </c>
-      <c r="B3" t="str">
-        <v>ANGIOCOR</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Dra. Venier</v>
-      </c>
-      <c r="D3" t="str">
-        <v>MARIA SILVA</v>
-      </c>
-      <c r="E3" t="str">
-        <v>87654321</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="str">
-        <v/>
-      </c>
-      <c r="H3" t="str">
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L3"/>
+    <ignoredError sqref="A1:L1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>